<commit_message>
Update PDF processing script to correctly extract month from filenames
Fixes an issue in the `process_ccc_pdfs_fixed.py` script where the month was not being correctly extracted from PDF filenames for statement month calculation.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 46cb15e0-d767-454a-946f-faa7b4e5437a
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 3f67af37-f64e-426d-b973-5286506a8521
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/6020cca9-a8d9-41a4-b1b0-5f1ba22a7012/46cb15e0-d767-454a-946f-faa7b4e5437a/hBg1LNV
</commit_message>
<xml_diff>
--- a/reports/CCC_Detailed_Reports/CCC_Final_Settlement_Report.xlsx
+++ b/reports/CCC_Detailed_Reports/CCC_Final_Settlement_Report.xlsx
@@ -8,11 +8,13 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="最终结算报告" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alliance Bank" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HSBC" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hong Leong Bank" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Maybank" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UOB" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alliance" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alliance Bank" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HLB" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HSBC" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hong Leong Bank" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Maybank" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UOB" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -524,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,7 +585,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2025-11-15 13:37:13</t>
+          <t>2025-11-15 13:53:14</t>
         </is>
       </c>
     </row>
@@ -595,7 +597,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>63条</t>
+          <t>69条</t>
         </is>
       </c>
     </row>
@@ -2739,146 +2741,344 @@
         <v>8099.129999999996</v>
       </c>
     </row>
-    <row r="74"/>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Alliance</t>
+        </is>
+      </c>
+      <c r="C74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="75">
-      <c r="A75" s="6" t="inlineStr">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Alliance Bank</t>
+        </is>
+      </c>
+      <c r="C75" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>HLB</t>
+        </is>
+      </c>
+      <c r="C76" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Hong Leong Bank</t>
+        </is>
+      </c>
+      <c r="C77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Maybank</t>
+        </is>
+      </c>
+      <c r="C78" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>UOB</t>
+        </is>
+      </c>
+      <c r="C79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80"/>
+    <row r="81">
+      <c r="A81" s="6" t="inlineStr">
         <is>
           <t>总计</t>
         </is>
       </c>
-      <c r="B75" s="6" t="inlineStr">
+      <c r="B81" s="6" t="inlineStr">
         <is>
           <t>所有银行</t>
         </is>
       </c>
-      <c r="C75" s="7" t="n">
+      <c r="C81" s="7" t="n">
         <v>334293.12</v>
       </c>
-      <c r="D75" s="7" t="n">
+      <c r="D81" s="7" t="n">
         <v>436323.08</v>
       </c>
-      <c r="E75" s="7" t="n">
+      <c r="E81" s="7" t="n">
         <v>-102029.96</v>
       </c>
-      <c r="F75" s="7" t="n">
+      <c r="F81" s="7" t="n">
         <v>536929</v>
       </c>
-      <c r="G75" s="7" t="n">
+      <c r="G81" s="7" t="n">
         <v>287262.98</v>
       </c>
-      <c r="H75" s="7" t="n">
+      <c r="H81" s="7" t="n">
         <v>249666.02</v>
       </c>
-      <c r="I75" s="7" t="n">
+      <c r="I81" s="7" t="n">
         <v>147636.06</v>
       </c>
     </row>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78" ht="25" customHeight="1">
-      <c r="A78" s="8" t="inlineStr">
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84" ht="25" customHeight="1">
+      <c r="A84" s="8" t="inlineStr">
         <is>
           <t>🎯 最终结算金额</t>
         </is>
       </c>
     </row>
-    <row r="79"/>
-    <row r="80">
-      <c r="A80" s="9" t="inlineStr">
+    <row r="85"/>
+    <row r="86">
+      <c r="A86" s="9" t="inlineStr">
         <is>
           <t>Owner账本:</t>
         </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>总消费:</t>
-        </is>
-      </c>
-      <c r="C81" s="10" t="n">
-        <v>334293.12</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>总付款:</t>
-        </is>
-      </c>
-      <c r="C82" s="10" t="n">
-        <v>436323.08</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" s="11" t="inlineStr">
-        <is>
-          <t>Owner OS Balance:</t>
-        </is>
-      </c>
-      <c r="C83" s="12" t="n">
-        <v>-102029.96</v>
-      </c>
-    </row>
-    <row r="84"/>
-    <row r="85">
-      <c r="A85" s="9" t="inlineStr">
-        <is>
-          <t>GZ账本:</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>GZ总消费 (Supplier):</t>
-        </is>
-      </c>
-      <c r="C86" s="10" t="n">
-        <v>536929</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
+          <t>总消费:</t>
+        </is>
+      </c>
+      <c r="C87" s="10" t="n">
+        <v>334293.12</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>总付款:</t>
+        </is>
+      </c>
+      <c r="C88" s="10" t="n">
+        <v>436323.08</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" s="11" t="inlineStr">
+        <is>
+          <t>Owner OS Balance:</t>
+        </is>
+      </c>
+      <c r="C89" s="12" t="n">
+        <v>-102029.96</v>
+      </c>
+    </row>
+    <row r="90"/>
+    <row r="91">
+      <c r="A91" s="9" t="inlineStr">
+        <is>
+          <t>GZ账本:</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>GZ总消费 (Supplier):</t>
+        </is>
+      </c>
+      <c r="C92" s="10" t="n">
+        <v>536929</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="inlineStr">
+        <is>
           <t>GZ总付款:</t>
         </is>
       </c>
-      <c r="C87" s="10" t="n">
+      <c r="C93" s="10" t="n">
         <v>287262.98</v>
       </c>
     </row>
-    <row r="88">
-      <c r="B88" s="11" t="inlineStr">
+    <row r="94">
+      <c r="B94" s="11" t="inlineStr">
         <is>
           <t>GZ OS Balance:</t>
         </is>
       </c>
-      <c r="C88" s="13" t="n">
+      <c r="C94" s="13" t="n">
         <v>249666.02</v>
       </c>
     </row>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91" ht="30" customHeight="1">
-      <c r="A91" s="14" t="inlineStr">
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97" ht="30" customHeight="1">
+      <c r="A97" s="14" t="inlineStr">
         <is>
           <t>INFINITE GZ 应支付给 OWNER:</t>
         </is>
       </c>
     </row>
-    <row r="92" ht="40" customHeight="1">
-      <c r="A92" s="15" t="n">
+    <row r="98" ht="40" customHeight="1">
+      <c r="A98" s="15" t="n">
         <v>249666.02</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A97:C97"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="A78:I78"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2890,7 +3090,146 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="16" t="inlineStr">
+        <is>
+          <t>Alliance - 月度明细</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>月份</t>
+        </is>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
+        <is>
+          <t>Owner消费</t>
+        </is>
+      </c>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Owner付款</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>Owner OS</t>
+        </is>
+      </c>
+      <c r="E3" s="17" t="inlineStr">
+        <is>
+          <t>GZ消费</t>
+        </is>
+      </c>
+      <c r="F3" s="17" t="inlineStr">
+        <is>
+          <t>GZ付款</t>
+        </is>
+      </c>
+      <c r="G3" s="17" t="inlineStr">
+        <is>
+          <t>GZ OS</t>
+        </is>
+      </c>
+      <c r="H3" s="17" t="inlineStr">
+        <is>
+          <t>月度净增</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>Alliance 小计</t>
+        </is>
+      </c>
+      <c r="B6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3294,32 +3633,60 @@
         <v>4099.3</v>
       </c>
     </row>
-    <row r="16"/>
-    <row r="17">
-      <c r="A17" s="11" t="inlineStr">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17"/>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
         <is>
           <t>Alliance Bank 小计</t>
         </is>
       </c>
-      <c r="B17" s="18" t="n">
+      <c r="B18" s="18" t="n">
         <v>25362.83</v>
       </c>
-      <c r="C17" s="18" t="n">
+      <c r="C18" s="18" t="n">
         <v>40904.42</v>
       </c>
-      <c r="D17" s="18" t="n">
+      <c r="D18" s="18" t="n">
         <v>-15541.59</v>
       </c>
-      <c r="E17" s="18" t="n">
+      <c r="E18" s="18" t="n">
         <v>29298</v>
       </c>
-      <c r="F17" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18" t="n">
+      <c r="F18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18" t="n">
         <v>29298</v>
       </c>
-      <c r="H17" s="18" t="n">
+      <c r="H18" s="18" t="n">
         <v>13756.41</v>
       </c>
     </row>
@@ -3331,7 +3698,146 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="16" t="inlineStr">
+        <is>
+          <t>HLB - 月度明细</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="17" t="inlineStr">
+        <is>
+          <t>月份</t>
+        </is>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
+        <is>
+          <t>Owner消费</t>
+        </is>
+      </c>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Owner付款</t>
+        </is>
+      </c>
+      <c r="D3" s="17" t="inlineStr">
+        <is>
+          <t>Owner OS</t>
+        </is>
+      </c>
+      <c r="E3" s="17" t="inlineStr">
+        <is>
+          <t>GZ消费</t>
+        </is>
+      </c>
+      <c r="F3" s="17" t="inlineStr">
+        <is>
+          <t>GZ付款</t>
+        </is>
+      </c>
+      <c r="G3" s="17" t="inlineStr">
+        <is>
+          <t>GZ OS</t>
+        </is>
+      </c>
+      <c r="H3" s="17" t="inlineStr">
+        <is>
+          <t>月度净增</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>HLB 小计</t>
+        </is>
+      </c>
+      <c r="B6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3778,13 +4284,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4216,32 +4722,60 @@
         <v>-2825.21</v>
       </c>
     </row>
-    <row r="17"/>
-    <row r="18">
-      <c r="A18" s="11" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
         <is>
           <t>Hong Leong Bank 小计</t>
         </is>
       </c>
-      <c r="B18" s="18" t="n">
+      <c r="B19" s="18" t="n">
         <v>68309.21000000001</v>
       </c>
-      <c r="C18" s="18" t="n">
+      <c r="C19" s="18" t="n">
         <v>136695.34</v>
       </c>
-      <c r="D18" s="18" t="n">
+      <c r="D19" s="18" t="n">
         <v>-68386.13</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E19" s="18" t="n">
         <v>246104</v>
       </c>
-      <c r="F18" s="18" t="n">
+      <c r="F19" s="18" t="n">
         <v>102753.52</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G19" s="18" t="n">
         <v>143350.48</v>
       </c>
-      <c r="H18" s="18" t="n">
+      <c r="H19" s="18" t="n">
         <v>74964.35000000001</v>
       </c>
     </row>
@@ -4253,13 +4787,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4691,32 +5225,60 @@
         <v>8099.129999999996</v>
       </c>
     </row>
-    <row r="17"/>
-    <row r="18">
-      <c r="A18" s="11" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
         <is>
           <t>Maybank 小计</t>
         </is>
       </c>
-      <c r="B18" s="18" t="n">
+      <c r="B19" s="18" t="n">
         <v>73727.00999999999</v>
       </c>
-      <c r="C18" s="18" t="n">
+      <c r="C19" s="18" t="n">
         <v>258723.32</v>
       </c>
-      <c r="D18" s="18" t="n">
+      <c r="D19" s="18" t="n">
         <v>-184996.31</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E19" s="18" t="n">
         <v>261527</v>
       </c>
-      <c r="F18" s="18" t="n">
+      <c r="F19" s="18" t="n">
         <v>53693.02</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G19" s="18" t="n">
         <v>207833.98</v>
       </c>
-      <c r="H18" s="18" t="n">
+      <c r="H19" s="18" t="n">
         <v>22837.66999999999</v>
       </c>
     </row>
@@ -4728,13 +5290,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5166,32 +5728,60 @@
         <v>-224.44</v>
       </c>
     </row>
-    <row r="17"/>
-    <row r="18">
-      <c r="A18" s="11" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
         <is>
           <t>UOB 小计</t>
         </is>
       </c>
-      <c r="B18" s="18" t="n">
+      <c r="B19" s="18" t="n">
         <v>87375.13</v>
       </c>
-      <c r="C18" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18" t="n">
+      <c r="C19" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="18" t="n">
         <v>87375.13</v>
       </c>
-      <c r="E18" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="18" t="n">
+      <c r="E19" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="18" t="n">
         <v>69807.91</v>
       </c>
-      <c r="G18" s="18" t="n">
+      <c r="G19" s="18" t="n">
         <v>-69807.91</v>
       </c>
-      <c r="H18" s="18" t="n">
+      <c r="H19" s="18" t="n">
         <v>17567.22</v>
       </c>
     </row>

</xml_diff>